<commit_message>
changes made on 14th June 2017
</commit_message>
<xml_diff>
--- a/MasterTestDataFile.xlsx
+++ b/MasterTestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Nicole&amp;2009</t>
+  </si>
+  <si>
+    <t>testSuccesfulLogOut</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:C734"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -455,14 +458,26 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>

</xml_diff>